<commit_message>
Add more tests for the retry loop logic in ElevatorController
</commit_message>
<xml_diff>
--- a/Metadata/Truthtable unit test ElevatorController.xlsx
+++ b/Metadata/Truthtable unit test ElevatorController.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\CVs etc\DVT\ElevatorAction\ElevatorAction\Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910982A7-149B-4A20-B6AC-B0CCC299C9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A840C10-34AD-49BF-B6A3-C6DE1E74C75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28692" yWindow="6660" windowWidth="23256" windowHeight="12456" xr2:uid="{5EDC8A44-778A-42DA-BB1E-D28BFB5AFFFC}"/>
+    <workbookView xWindow="40224" yWindow="7080" windowWidth="11712" windowHeight="12336" xr2:uid="{5EDC8A44-778A-42DA-BB1E-D28BFB5AFFFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Config retryCount</t>
   </si>
@@ -50,6 +50,9 @@
     <t>Return value</t>
   </si>
   <si>
+    <t>&gt; 0</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -62,18 +65,6 @@
     <t>&gt; max retries</t>
   </si>
   <si>
-    <t>&gt; 1</t>
-  </si>
-  <si>
-    <t>&gt; 2</t>
-  </si>
-  <si>
-    <t>&gt; 3</t>
-  </si>
-  <si>
-    <t>&gt; 0*</t>
-  </si>
-  <si>
     <t>none (keeps retrying)</t>
   </si>
   <si>
@@ -92,29 +83,40 @@
     <t>ElevatorControllerTests.GetCommandAfterRetry_NoRetryMax_ReturnsValidCommandAfterManyTries</t>
   </si>
   <si>
-    <t>See above; we can't create a test that never stops looping but above tests 20 retries before valid command</t>
-  </si>
-  <si>
-    <t>abort</t>
-  </si>
-  <si>
     <t>abort (after retryCount attempts)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Validation method should prevent this scenario, but if it happens, it should return </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>abort</t>
-    </r>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>We can't create a test that never stops looping but above tests 20 retries before valid command</t>
+  </si>
+  <si>
+    <t>ElevatorControllerTests.GetCommandAfterRetry_RetryMaxZero_Aborts</t>
+  </si>
+  <si>
+    <t>ElevatorControllerTests.GetCommandAfterRetry_WithinRetryLimit_ReturnsCommand</t>
+  </si>
+  <si>
+    <t>ElevatorControllerTests.GetCommandAfterRetry_WithinRetryLimitWithInvalidCommand_ReturnsAbort</t>
+  </si>
+  <si>
+    <t>ElevatorControllerTests.GetCommandAfterRetry_ReachedRetryLimit_ReturnsValidCommand</t>
+  </si>
+  <si>
+    <t>ElevatorControllerTests.GetCommandAfterRetry_ReachedRetryLimitWithInvalidCommand_ReturnsAbort</t>
+  </si>
+  <si>
+    <t>abort (after exactly retryCount attempts)</t>
+  </si>
+  <si>
+    <t>ElevatorControllerTests.GetCommandAfterRetry_ExceedRetryLimit_ReturnsAbort</t>
+  </si>
+  <si>
+    <t>Throws ArgumentException</t>
+  </si>
+  <si>
+    <t>Validation method should prevent this scenario, but if it happens, throw an exception</t>
   </si>
 </sst>
 </file>
@@ -152,15 +154,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -183,11 +191,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -208,6 +229,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -544,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E0A1B5-34F0-4E6B-93A5-F40FDAA226FD}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,16 +601,16 @@
     <col min="2" max="2" width="14.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.21875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="88.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="6" width="97" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,120 +623,160 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="B8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="6"/>
+      <c r="D11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>